<commit_message>
1.SpriteLoaderToABSpriteLoader.cs脚本，将场景中的SpriteLoader脚本全部替换成ABSpriteLoader脚本。 2.SpriteLoader.cs脚本，SetAll，SetImageBox，SetImageName等方法设置成public的。 3.TextureLoader.cs脚本，SetAll，SetImageBox，SetImageName等方法设置成public的。 4.ABSpriteLoader.cs脚本，从assetbundle中取sprite。 5.CyclingView.cs脚本，头像改为从assetbundle中获取。 6.BasePlayer.cs脚本，头像改为从assetbundle中获取。 7.ScenicCard.cs脚本，景点图片改为从assetbundle中获取。 8.CommonImageUtils.cs脚本，改为记录头像id与文件名的关联。 9.Cycling_2.prefab预制体，场景中的SpriteLoader脚本全部替换成ABSpriteLoader脚本。
</commit_message>
<xml_diff>
--- a/Resources/configs/ConfigBuilder.xlsx
+++ b/Resources/configs/ConfigBuilder.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="20730" windowHeight="11760" tabRatio="749"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="20730" windowHeight="11760" tabRatio="749" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Item" sheetId="33" r:id="rId1"/>
@@ -493,7 +493,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="663" uniqueCount="321">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="663" uniqueCount="315">
   <si>
     <t>Image</t>
     <phoneticPr fontId="4" type="noConversion"/>
@@ -968,33 +968,6 @@
     <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
-    <t>NanJing/card_nanjing01</t>
-  </si>
-  <si>
-    <t>NanJing/card_nanjing02</t>
-  </si>
-  <si>
-    <t>NanJing/card_nanjing03</t>
-  </si>
-  <si>
-    <t>NanJing/card_nanjing04</t>
-  </si>
-  <si>
-    <t>NanJing/card_nanjing05</t>
-  </si>
-  <si>
-    <t>NanJing/card_nanjing06</t>
-  </si>
-  <si>
-    <t>NanJing/card_nanjing07</t>
-  </si>
-  <si>
-    <t>NanJing/card_nanjing08</t>
-  </si>
-  <si>
-    <t>NanJing/card_nanjing09</t>
-  </si>
-  <si>
     <t>arrow_panel</t>
   </si>
   <si>
@@ -1180,25 +1153,6 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>ZhenJiang/card_zhenjiang01</t>
-    <phoneticPr fontId="10" type="noConversion"/>
-  </si>
-  <si>
-    <t>ZhenJiang/card_zhenjiang02</t>
-  </si>
-  <si>
-    <t>ZhenJiang/card_zhenjiang03</t>
-  </si>
-  <si>
-    <t>ZhenJiang/card_zhenjiang04</t>
-  </si>
-  <si>
-    <t>ZhenJiang/card_zhenjiang05</t>
-  </si>
-  <si>
-    <t>ZhenJiang/card_zhenjiang06</t>
-  </si>
-  <si>
     <t>card_zhenjiang01</t>
   </si>
   <si>
@@ -1664,6 +1618,33 @@
   <si>
     <t>ticket_normal</t>
     <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>card_nanjing01</t>
+  </si>
+  <si>
+    <t>card_nanjing02</t>
+  </si>
+  <si>
+    <t>card_nanjing03</t>
+  </si>
+  <si>
+    <t>card_nanjing04</t>
+  </si>
+  <si>
+    <t>card_nanjing05</t>
+  </si>
+  <si>
+    <t>card_nanjing06</t>
+  </si>
+  <si>
+    <t>card_nanjing07</t>
+  </si>
+  <si>
+    <t>card_nanjing08</t>
+  </si>
+  <si>
+    <t>card_nanjing09</t>
   </si>
 </sst>
 </file>
@@ -2376,7 +2357,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
@@ -2394,19 +2375,19 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="21" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="B1" s="21" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="C1" s="21" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="D1" s="21" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="E1" s="21" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="F1" s="21" t="s">
         <v>44</v>
@@ -2414,19 +2395,19 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="16" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="F2" s="10" t="s">
         <v>57</v>
@@ -2440,7 +2421,7 @@
         <v>10</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="E3" s="6"/>
       <c r="F3" s="10" t="str">
@@ -2731,7 +2712,7 @@
   <dimension ref="A1:J96"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D18" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="D27" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight" activeCell="B31" sqref="B31"/>
@@ -3758,7 +3739,7 @@
         <v>3</v>
       </c>
       <c r="D40" s="10" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
       <c r="E40" s="10" t="s">
         <v>64</v>
@@ -3767,7 +3748,7 @@
         <v>63</v>
       </c>
       <c r="G40" s="10" t="s">
-        <v>202</v>
+        <v>187</v>
       </c>
       <c r="I40" s="15">
         <v>1</v>
@@ -3782,7 +3763,7 @@
         <v>3</v>
       </c>
       <c r="D41" s="10" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="E41" s="10" t="s">
         <v>64</v>
@@ -3791,7 +3772,7 @@
         <v>63</v>
       </c>
       <c r="G41" s="10" t="s">
-        <v>202</v>
+        <v>187</v>
       </c>
       <c r="I41" s="15">
         <v>1</v>
@@ -3806,7 +3787,7 @@
         <v>3</v>
       </c>
       <c r="D42" s="10" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="E42" s="10" t="s">
         <v>64</v>
@@ -3815,7 +3796,7 @@
         <v>63</v>
       </c>
       <c r="G42" s="10" t="s">
-        <v>202</v>
+        <v>187</v>
       </c>
       <c r="I42" s="15">
         <v>1</v>
@@ -3830,7 +3811,7 @@
         <v>3</v>
       </c>
       <c r="D43" s="10" t="s">
-        <v>199</v>
+        <v>184</v>
       </c>
       <c r="E43" s="10" t="s">
         <v>64</v>
@@ -3839,7 +3820,7 @@
         <v>63</v>
       </c>
       <c r="G43" s="10" t="s">
-        <v>202</v>
+        <v>187</v>
       </c>
       <c r="I43" s="15">
         <v>1</v>
@@ -3854,7 +3835,7 @@
         <v>3</v>
       </c>
       <c r="D44" s="10" t="s">
-        <v>200</v>
+        <v>185</v>
       </c>
       <c r="E44" s="10" t="s">
         <v>64</v>
@@ -3863,7 +3844,7 @@
         <v>63</v>
       </c>
       <c r="G44" s="10" t="s">
-        <v>202</v>
+        <v>187</v>
       </c>
       <c r="I44" s="15">
         <v>1</v>
@@ -3878,7 +3859,7 @@
         <v>3</v>
       </c>
       <c r="D45" s="10" t="s">
-        <v>201</v>
+        <v>186</v>
       </c>
       <c r="E45" s="10" t="s">
         <v>64</v>
@@ -3887,7 +3868,7 @@
         <v>63</v>
       </c>
       <c r="G45" s="10" t="s">
-        <v>202</v>
+        <v>187</v>
       </c>
       <c r="I45" s="15">
         <v>1</v>
@@ -3902,7 +3883,7 @@
         <v>3</v>
       </c>
       <c r="D46" s="10" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="E46" s="10" t="s">
         <v>64</v>
@@ -3974,7 +3955,7 @@
         <v>3</v>
       </c>
       <c r="D49" s="10" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="E49" s="10" t="s">
         <v>64</v>
@@ -4118,7 +4099,7 @@
         <v>3</v>
       </c>
       <c r="D55" s="10" t="s">
-        <v>311</v>
+        <v>296</v>
       </c>
       <c r="E55" s="10" t="s">
         <v>64</v>
@@ -4142,7 +4123,7 @@
         <v>3</v>
       </c>
       <c r="D56" s="10" t="s">
-        <v>312</v>
+        <v>297</v>
       </c>
       <c r="E56" s="10" t="s">
         <v>64</v>
@@ -4166,7 +4147,7 @@
         <v>3</v>
       </c>
       <c r="D57" s="10" t="s">
-        <v>307</v>
+        <v>292</v>
       </c>
       <c r="E57" s="10" t="s">
         <v>64</v>
@@ -4190,7 +4171,7 @@
         <v>3</v>
       </c>
       <c r="D58" s="10" t="s">
-        <v>308</v>
+        <v>293</v>
       </c>
       <c r="E58" s="10" t="s">
         <v>64</v>
@@ -4214,7 +4195,7 @@
         <v>3</v>
       </c>
       <c r="D59" s="10" t="s">
-        <v>309</v>
+        <v>294</v>
       </c>
       <c r="E59" s="10" t="s">
         <v>64</v>
@@ -4238,7 +4219,7 @@
         <v>3</v>
       </c>
       <c r="D60" s="10" t="s">
-        <v>310</v>
+        <v>295</v>
       </c>
       <c r="E60" s="10" t="s">
         <v>64</v>
@@ -4262,7 +4243,7 @@
         <v>3</v>
       </c>
       <c r="D61" s="10" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="E61" s="10" t="s">
         <v>64</v>
@@ -4358,7 +4339,7 @@
         <v>3</v>
       </c>
       <c r="D65" s="10" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="E65" s="10" t="s">
         <v>64</v>
@@ -4382,7 +4363,7 @@
         <v>3</v>
       </c>
       <c r="D66" s="10" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="E66" s="10" t="s">
         <v>64</v>
@@ -4406,7 +4387,7 @@
         <v>3</v>
       </c>
       <c r="D67" s="10" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="E67" s="10" t="s">
         <v>64</v>
@@ -4478,7 +4459,7 @@
         <v>3</v>
       </c>
       <c r="D70" s="10" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="E70" s="10" t="s">
         <v>64</v>
@@ -4502,7 +4483,7 @@
         <v>3</v>
       </c>
       <c r="D71" s="10" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="E71" s="10" t="s">
         <v>64</v>
@@ -4526,7 +4507,7 @@
         <v>3</v>
       </c>
       <c r="D72" s="10" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="E72" s="10" t="s">
         <v>64</v>
@@ -4550,7 +4531,7 @@
         <v>3</v>
       </c>
       <c r="D73" s="10" t="s">
-        <v>316</v>
+        <v>301</v>
       </c>
       <c r="E73" s="10" t="s">
         <v>64</v>
@@ -4646,7 +4627,7 @@
         <v>3</v>
       </c>
       <c r="D77" s="10" t="s">
-        <v>314</v>
+        <v>299</v>
       </c>
       <c r="E77" s="10" t="s">
         <v>64</v>
@@ -4790,7 +4771,7 @@
         <v>3</v>
       </c>
       <c r="D83" s="10" t="s">
-        <v>317</v>
+        <v>302</v>
       </c>
       <c r="E83" s="10" t="s">
         <v>64</v>
@@ -4814,7 +4795,7 @@
         <v>3</v>
       </c>
       <c r="D84" s="10" t="s">
-        <v>318</v>
+        <v>303</v>
       </c>
       <c r="E84" s="10" t="s">
         <v>64</v>
@@ -4838,7 +4819,7 @@
         <v>3</v>
       </c>
       <c r="D85" s="10" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="E85" s="10" t="s">
         <v>64</v>
@@ -4862,7 +4843,7 @@
         <v>3</v>
       </c>
       <c r="D86" s="10" t="s">
-        <v>319</v>
+        <v>304</v>
       </c>
       <c r="E86" s="10" t="s">
         <v>64</v>
@@ -4886,7 +4867,7 @@
         <v>3</v>
       </c>
       <c r="D87" s="10" t="s">
-        <v>320</v>
+        <v>305</v>
       </c>
       <c r="E87" s="10" t="s">
         <v>64</v>
@@ -4934,7 +4915,7 @@
         <v>3</v>
       </c>
       <c r="D89" s="10" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="E89" s="10" t="s">
         <v>64</v>
@@ -4982,7 +4963,7 @@
         <v>3</v>
       </c>
       <c r="D91" s="10" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="E91" s="10" t="s">
         <v>64</v>
@@ -5006,7 +4987,7 @@
         <v>3</v>
       </c>
       <c r="D92" s="10" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="E92" s="10" t="s">
         <v>64</v>
@@ -5030,7 +5011,7 @@
         <v>3</v>
       </c>
       <c r="D93" s="10" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="E93" s="10" t="s">
         <v>64</v>
@@ -5054,7 +5035,7 @@
         <v>3</v>
       </c>
       <c r="D94" s="10" t="s">
-        <v>313</v>
+        <v>298</v>
       </c>
       <c r="E94" s="10" t="s">
         <v>64</v>
@@ -5078,7 +5059,7 @@
         <v>3</v>
       </c>
       <c r="D95" s="10" t="s">
-        <v>315</v>
+        <v>300</v>
       </c>
       <c r="E95" s="10" t="s">
         <v>64</v>
@@ -5303,19 +5284,19 @@
         <v>12</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>203</v>
+        <v>188</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>206</v>
+        <v>191</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>207</v>
+        <v>192</v>
       </c>
       <c r="L1" s="3"/>
       <c r="M1" s="2" t="s">
@@ -5353,19 +5334,19 @@
         <v>36</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>204</v>
+        <v>189</v>
       </c>
       <c r="K2" s="6" t="s">
-        <v>205</v>
+        <v>190</v>
       </c>
       <c r="M2" s="6" t="s">
         <v>40</v>
@@ -5391,10 +5372,10 @@
         <v>14</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="I3" s="6">
         <v>3202</v>
@@ -5415,25 +5396,25 @@
         <v>3202</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="C4" s="6">
         <v>32</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="E4" s="6">
         <v>3202</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="J4" s="6">
         <v>18</v>
@@ -5657,7 +5638,7 @@
         <v>320201</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="C12" s="6">
         <v>3202</v>
@@ -5672,7 +5653,7 @@
         <v>320202</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
       <c r="C13" s="6">
         <v>3202</v>
@@ -5687,7 +5668,7 @@
         <v>320203</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="C14" s="6">
         <v>3202</v>
@@ -5702,7 +5683,7 @@
         <v>320204</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="C15" s="6">
         <v>3202</v>
@@ -5717,7 +5698,7 @@
         <v>320205</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="C16" s="6">
         <v>3202</v>
@@ -5732,7 +5713,7 @@
         <v>320206</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
       <c r="C17" s="6">
         <v>3202</v>
@@ -5757,12 +5738,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:S20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="4" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
       <selection activeCell="C222" sqref="C222:C228"/>
       <selection pane="topRight" activeCell="C222" sqref="C222:C228"/>
       <selection pane="bottomLeft" activeCell="C222" sqref="C222:C228"/>
-      <selection pane="bottomRight" activeCell="A3" sqref="A3:A17"/>
+      <selection pane="bottomRight" activeCell="E3" sqref="E3:E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12"/>
@@ -5779,10 +5760,10 @@
   <sheetData>
     <row r="1" spans="1:19" s="5" customFormat="1">
       <c r="A1" s="1" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>7</v>
@@ -5797,7 +5778,7 @@
         <v>6</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>208</v>
+        <v>193</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>28</v>
@@ -5816,16 +5797,16 @@
     </row>
     <row r="2" spans="1:19">
       <c r="A2" s="19" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="E2" s="7" t="s">
         <v>0</v>
@@ -5834,7 +5815,7 @@
         <v>8</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>208</v>
+        <v>193</v>
       </c>
       <c r="H2" s="7" t="s">
         <v>4</v>
@@ -5842,10 +5823,10 @@
     </row>
     <row r="3" spans="1:19">
       <c r="A3" s="18" t="s">
-        <v>292</v>
+        <v>277</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>16</v>
@@ -5854,26 +5835,26 @@
         <v>320101</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>131</v>
+        <v>306</v>
       </c>
       <c r="F3" s="8" t="str">
         <f>C3&amp;"介绍"</f>
         <v>中山陵介绍</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>209</v>
+        <v>194</v>
       </c>
       <c r="H3" s="6" t="str">
         <f>"&lt;Card CardID="""&amp;A3&amp;""" CardType="""&amp;B3&amp;""" CardName="""&amp;C3&amp;""" ScenicID="""&amp;D3&amp;""" Image="""&amp;E3&amp;""" Text="""&amp;F3&amp;""" Url="""&amp;G3&amp;""" /&gt;"</f>
-        <v>&lt;Card CardID="20010001" CardType="01" CardName="中山陵" ScenicID="320101" Image="NanJing/card_nanjing01" Text="中山陵介绍" Url="https://baike.baidu.com/item/%E4%B8%AD%E5%B1%B1%E9%99%B5/246397" /&gt;</v>
+        <v>&lt;Card CardID="20010001" CardType="01" CardName="中山陵" ScenicID="320101" Image="card_nanjing01" Text="中山陵介绍" Url="https://baike.baidu.com/item/%E4%B8%AD%E5%B1%B1%E9%99%B5/246397" /&gt;</v>
       </c>
     </row>
     <row r="4" spans="1:19">
       <c r="A4" s="18" t="s">
-        <v>293</v>
+        <v>278</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>17</v>
@@ -5882,26 +5863,26 @@
         <v>320102</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>132</v>
+        <v>307</v>
       </c>
       <c r="F4" s="8" t="str">
         <f t="shared" ref="F4:F17" si="0">C4&amp;"介绍"</f>
         <v>总统府介绍</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>210</v>
+        <v>195</v>
       </c>
       <c r="H4" s="6" t="str">
         <f t="shared" ref="H4:H17" si="1">"&lt;Card CardID="""&amp;A4&amp;""" CardType="""&amp;B4&amp;""" CardName="""&amp;C4&amp;""" ScenicID="""&amp;D4&amp;""" Image="""&amp;E4&amp;""" Text="""&amp;F4&amp;""" Url="""&amp;G4&amp;""" /&gt;"</f>
-        <v>&lt;Card CardID="20010002" CardType="01" CardName="总统府" ScenicID="320102" Image="NanJing/card_nanjing02" Text="总统府介绍" Url="https://baike.baidu.com/item/%E5%8D%97%E4%BA%AC%E6%80%BB%E7%BB%9F%E5%BA%9C/3027343?fromtitle=%E6%80%BB%E7%BB%9F%E5%BA%9C&amp;fromid=18727656" /&gt;</v>
+        <v>&lt;Card CardID="20010002" CardType="01" CardName="总统府" ScenicID="320102" Image="card_nanjing02" Text="总统府介绍" Url="https://baike.baidu.com/item/%E5%8D%97%E4%BA%AC%E6%80%BB%E7%BB%9F%E5%BA%9C/3027343?fromtitle=%E6%80%BB%E7%BB%9F%E5%BA%9C&amp;fromid=18727656" /&gt;</v>
       </c>
     </row>
     <row r="5" spans="1:19">
       <c r="A5" s="18" t="s">
-        <v>294</v>
+        <v>279</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>18</v>
@@ -5910,26 +5891,26 @@
         <v>320103</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>133</v>
+        <v>308</v>
       </c>
       <c r="F5" s="8" t="str">
         <f t="shared" si="0"/>
         <v>夫子庙介绍</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>211</v>
+        <v>196</v>
       </c>
       <c r="H5" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;Card CardID="20010003" CardType="01" CardName="夫子庙" ScenicID="320103" Image="NanJing/card_nanjing03" Text="夫子庙介绍" Url="https://baike.baidu.com/item/%E5%8D%97%E4%BA%AC%E5%A4%AB%E5%AD%90%E5%BA%99/510169?fromtitle=%E5%A4%AB%E5%AD%90%E5%BA%99&amp;fromid=978934" /&gt;</v>
+        <v>&lt;Card CardID="20010003" CardType="01" CardName="夫子庙" ScenicID="320103" Image="card_nanjing03" Text="夫子庙介绍" Url="https://baike.baidu.com/item/%E5%8D%97%E4%BA%AC%E5%A4%AB%E5%AD%90%E5%BA%99/510169?fromtitle=%E5%A4%AB%E5%AD%90%E5%BA%99&amp;fromid=978934" /&gt;</v>
       </c>
     </row>
     <row r="6" spans="1:19">
       <c r="A6" s="18" t="s">
-        <v>295</v>
+        <v>280</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>19</v>
@@ -5938,26 +5919,26 @@
         <v>320104</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>134</v>
+        <v>309</v>
       </c>
       <c r="F6" s="8" t="str">
         <f t="shared" si="0"/>
         <v>瞻园介绍</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>212</v>
+        <v>197</v>
       </c>
       <c r="H6" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;Card CardID="20010004" CardType="01" CardName="瞻园" ScenicID="320104" Image="NanJing/card_nanjing04" Text="瞻园介绍" Url="https://baike.baidu.com/item/%E8%A9%B9%E5%9B%AD" /&gt;</v>
+        <v>&lt;Card CardID="20010004" CardType="01" CardName="瞻园" ScenicID="320104" Image="card_nanjing04" Text="瞻园介绍" Url="https://baike.baidu.com/item/%E8%A9%B9%E5%9B%AD" /&gt;</v>
       </c>
     </row>
     <row r="7" spans="1:19">
       <c r="A7" s="18" t="s">
-        <v>296</v>
+        <v>281</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>20</v>
@@ -5966,26 +5947,26 @@
         <v>320105</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>135</v>
+        <v>310</v>
       </c>
       <c r="F7" s="8" t="str">
         <f t="shared" si="0"/>
         <v>玄武湖公园介绍</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>213</v>
+        <v>198</v>
       </c>
       <c r="H7" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;Card CardID="20010005" CardType="01" CardName="玄武湖公园" ScenicID="320105" Image="NanJing/card_nanjing05" Text="玄武湖公园介绍" Url="https://baike.baidu.com/item/%E7%8E%84%E6%AD%A6%E6%B9%96?fromtitle=%E7%8E%84%E6%AD%A6%E6%B9%96%E5%85%AC%E5%9B%AD&amp;fromid=217739" /&gt;</v>
+        <v>&lt;Card CardID="20010005" CardType="01" CardName="玄武湖公园" ScenicID="320105" Image="card_nanjing05" Text="玄武湖公园介绍" Url="https://baike.baidu.com/item/%E7%8E%84%E6%AD%A6%E6%B9%96?fromtitle=%E7%8E%84%E6%AD%A6%E6%B9%96%E5%85%AC%E5%9B%AD&amp;fromid=217739" /&gt;</v>
       </c>
     </row>
     <row r="8" spans="1:19">
       <c r="A8" s="18" t="s">
-        <v>297</v>
+        <v>282</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>21</v>
@@ -5994,26 +5975,26 @@
         <v>320106</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>136</v>
+        <v>311</v>
       </c>
       <c r="F8" s="8" t="str">
         <f t="shared" si="0"/>
         <v>明孝陵介绍</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>214</v>
+        <v>199</v>
       </c>
       <c r="H8" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;Card CardID="20010006" CardType="01" CardName="明孝陵" ScenicID="320106" Image="NanJing/card_nanjing06" Text="明孝陵介绍" Url="https://baike.baidu.com/item/%E6%98%8E%E5%AD%9D%E9%99%B5/751826" /&gt;</v>
+        <v>&lt;Card CardID="20010006" CardType="01" CardName="明孝陵" ScenicID="320106" Image="card_nanjing06" Text="明孝陵介绍" Url="https://baike.baidu.com/item/%E6%98%8E%E5%AD%9D%E9%99%B5/751826" /&gt;</v>
       </c>
     </row>
     <row r="9" spans="1:19">
       <c r="A9" s="18" t="s">
-        <v>298</v>
+        <v>283</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>22</v>
@@ -6022,26 +6003,26 @@
         <v>320107</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>137</v>
+        <v>312</v>
       </c>
       <c r="F9" s="8" t="str">
         <f t="shared" si="0"/>
         <v>美龄宫介绍</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>215</v>
+        <v>200</v>
       </c>
       <c r="H9" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;Card CardID="20010007" CardType="01" CardName="美龄宫" ScenicID="320107" Image="NanJing/card_nanjing07" Text="美龄宫介绍" Url="https://baike.baidu.com/item/%E5%9B%BD%E6%B0%91%E6%94%BF%E5%BA%9C%E4%B8%BB%E5%B8%AD%E5%AE%98%E9%82%B8%E6%97%A7%E5%9D%80?fromtitle=%E7%BE%8E%E9%BE%84%E5%AE%AB&amp;fromid=1173649" /&gt;</v>
+        <v>&lt;Card CardID="20010007" CardType="01" CardName="美龄宫" ScenicID="320107" Image="card_nanjing07" Text="美龄宫介绍" Url="https://baike.baidu.com/item/%E5%9B%BD%E6%B0%91%E6%94%BF%E5%BA%9C%E4%B8%BB%E5%B8%AD%E5%AE%98%E9%82%B8%E6%97%A7%E5%9D%80?fromtitle=%E7%BE%8E%E9%BE%84%E5%AE%AB&amp;fromid=1173649" /&gt;</v>
       </c>
     </row>
     <row r="10" spans="1:19">
       <c r="A10" s="18" t="s">
-        <v>299</v>
+        <v>284</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>24</v>
@@ -6050,26 +6031,26 @@
         <v>320108</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>138</v>
+        <v>313</v>
       </c>
       <c r="F10" s="8" t="str">
         <f t="shared" si="0"/>
         <v>南京大屠杀纪念馆介绍</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>216</v>
+        <v>201</v>
       </c>
       <c r="H10" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;Card CardID="20010008" CardType="01" CardName="南京大屠杀纪念馆" ScenicID="320108" Image="NanJing/card_nanjing08" Text="南京大屠杀纪念馆介绍" Url="https://baike.baidu.com/item/%E4%BE%B5%E5%8D%8E%E6%97%A5%E5%86%9B%E5%8D%97%E4%BA%AC%E5%A4%A7%E5%B1%A0%E6%9D%80%E9%81%87%E9%9A%BE%E5%90%8C%E8%83%9E%E7%BA%AA%E5%BF%B5%E9%A6%86" /&gt;</v>
+        <v>&lt;Card CardID="20010008" CardType="01" CardName="南京大屠杀纪念馆" ScenicID="320108" Image="card_nanjing08" Text="南京大屠杀纪念馆介绍" Url="https://baike.baidu.com/item/%E4%BE%B5%E5%8D%8E%E6%97%A5%E5%86%9B%E5%8D%97%E4%BA%AC%E5%A4%A7%E5%B1%A0%E6%9D%80%E9%81%87%E9%9A%BE%E5%90%8C%E8%83%9E%E7%BA%AA%E5%BF%B5%E9%A6%86" /&gt;</v>
       </c>
     </row>
     <row r="11" spans="1:19">
       <c r="A11" s="18" t="s">
-        <v>300</v>
+        <v>285</v>
       </c>
       <c r="B11" s="18" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="C11" s="6" t="s">
         <v>23</v>
@@ -6078,147 +6059,147 @@
         <v>320109</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>139</v>
+        <v>314</v>
       </c>
       <c r="F11" s="8" t="str">
         <f t="shared" si="0"/>
         <v>栖霞山介绍</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>217</v>
+        <v>202</v>
       </c>
       <c r="H11" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;Card CardID="20010009" CardType="01" CardName="栖霞山" ScenicID="320109" Image="NanJing/card_nanjing09" Text="栖霞山介绍" Url="https://baike.baidu.com/item/%E6%A0%96%E9%9C%9E%E5%B1%B1/151842" /&gt;</v>
+        <v>&lt;Card CardID="20010009" CardType="01" CardName="栖霞山" ScenicID="320109" Image="card_nanjing09" Text="栖霞山介绍" Url="https://baike.baidu.com/item/%E6%A0%96%E9%9C%9E%E5%B1%B1/151842" /&gt;</v>
       </c>
     </row>
     <row r="12" spans="1:19">
       <c r="A12" s="18" t="s">
-        <v>301</v>
+        <v>286</v>
       </c>
       <c r="B12" s="18" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="D12" s="6">
         <v>320201</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
       <c r="F12" s="8" t="str">
         <f t="shared" si="0"/>
         <v>西津渡古街介绍</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>218</v>
+        <v>203</v>
       </c>
       <c r="H12" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;Card CardID="20010010" CardType="01" CardName="西津渡古街" ScenicID="320201" Image="ZhenJiang/card_zhenjiang01" Text="西津渡古街介绍" Url="https://baike.baidu.com/item/%E8%A5%BF%E6%B4%A5%E6%B8%A1%E5%8F%A4%E8%A1%97/3265815?fr=aladdin" /&gt;</v>
+        <v>&lt;Card CardID="20010010" CardType="01" CardName="西津渡古街" ScenicID="320201" Image="card_zhenjiang01" Text="西津渡古街介绍" Url="https://baike.baidu.com/item/%E8%A5%BF%E6%B4%A5%E6%B8%A1%E5%8F%A4%E8%A1%97/3265815?fr=aladdin" /&gt;</v>
       </c>
     </row>
     <row r="13" spans="1:19">
       <c r="A13" s="18" t="s">
-        <v>302</v>
+        <v>287</v>
       </c>
       <c r="B13" s="18" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
       <c r="D13" s="6">
         <v>320202</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="F13" s="8" t="str">
         <f t="shared" si="0"/>
         <v>金山寺介绍</v>
       </c>
       <c r="G13" s="8" t="s">
-        <v>219</v>
+        <v>204</v>
       </c>
       <c r="H13" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;Card CardID="20010011" CardType="01" CardName="金山寺" ScenicID="320202" Image="ZhenJiang/card_zhenjiang02" Text="金山寺介绍" Url="https://baike.baidu.com/item/%E9%87%91%E5%B1%B1%E5%AF%BA/3942" /&gt;</v>
+        <v>&lt;Card CardID="20010011" CardType="01" CardName="金山寺" ScenicID="320202" Image="card_zhenjiang02" Text="金山寺介绍" Url="https://baike.baidu.com/item/%E9%87%91%E5%B1%B1%E5%AF%BA/3942" /&gt;</v>
       </c>
     </row>
     <row r="14" spans="1:19">
       <c r="A14" s="18" t="s">
-        <v>303</v>
+        <v>288</v>
       </c>
       <c r="B14" s="18" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="D14" s="6">
         <v>320203</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="F14" s="8" t="str">
         <f t="shared" si="0"/>
         <v>北固山介绍</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>220</v>
+        <v>205</v>
       </c>
       <c r="H14" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;Card CardID="20010012" CardType="01" CardName="北固山" ScenicID="320203" Image="ZhenJiang/card_zhenjiang03" Text="北固山介绍" Url="https://baike.baidu.com/item/%E5%8C%97%E5%9B%BA%E5%B1%B1/625922" /&gt;</v>
+        <v>&lt;Card CardID="20010012" CardType="01" CardName="北固山" ScenicID="320203" Image="card_zhenjiang03" Text="北固山介绍" Url="https://baike.baidu.com/item/%E5%8C%97%E5%9B%BA%E5%B1%B1/625922" /&gt;</v>
       </c>
     </row>
     <row r="15" spans="1:19">
       <c r="A15" s="18" t="s">
-        <v>304</v>
+        <v>289</v>
       </c>
       <c r="B15" s="18" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="D15" s="6">
         <v>320204</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="F15" s="8" t="str">
         <f t="shared" si="0"/>
         <v>焦山介绍</v>
       </c>
       <c r="G15" s="8" t="s">
-        <v>221</v>
+        <v>206</v>
       </c>
       <c r="H15" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;Card CardID="20010013" CardType="01" CardName="焦山" ScenicID="320204" Image="ZhenJiang/card_zhenjiang04" Text="焦山介绍" Url="https://baike.baidu.com/item/%E7%84%A6%E5%B1%B1%E9%A3%8E%E6%99%AF%E5%8C%BA/7985811?fromtitle=%E7%84%A6%E5%B1%B1&amp;fromid=922275" /&gt;</v>
+        <v>&lt;Card CardID="20010013" CardType="01" CardName="焦山" ScenicID="320204" Image="card_zhenjiang04" Text="焦山介绍" Url="https://baike.baidu.com/item/%E7%84%A6%E5%B1%B1%E9%A3%8E%E6%99%AF%E5%8C%BA/7985811?fromtitle=%E7%84%A6%E5%B1%B1&amp;fromid=922275" /&gt;</v>
       </c>
     </row>
     <row r="16" spans="1:19">
       <c r="A16" s="18" t="s">
-        <v>305</v>
+        <v>290</v>
       </c>
       <c r="B16" s="18" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="D16" s="6">
         <v>320205</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
       <c r="F16" s="8" t="str">
         <f t="shared" si="0"/>
@@ -6226,35 +6207,35 @@
       </c>
       <c r="H16" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;Card CardID="20010014" CardType="01" CardName="得撒石磨豆腐村" ScenicID="320205" Image="ZhenJiang/card_zhenjiang05" Text="得撒石磨豆腐村介绍" Url="" /&gt;</v>
+        <v>&lt;Card CardID="20010014" CardType="01" CardName="得撒石磨豆腐村" ScenicID="320205" Image="card_zhenjiang05" Text="得撒石磨豆腐村介绍" Url="" /&gt;</v>
       </c>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="18" t="s">
-        <v>306</v>
+        <v>291</v>
       </c>
       <c r="B17" s="18" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
       <c r="D17" s="6">
         <v>320206</v>
       </c>
       <c r="E17" s="10" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="F17" s="8" t="str">
         <f t="shared" si="0"/>
         <v>宝华山国家森林公园介绍</v>
       </c>
       <c r="G17" s="8" t="s">
-        <v>222</v>
+        <v>207</v>
       </c>
       <c r="H17" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;Card CardID="20010015" CardType="01" CardName="宝华山国家森林公园" ScenicID="320206" Image="ZhenJiang/card_zhenjiang06" Text="宝华山国家森林公园介绍" Url="https://baike.baidu.com/item/%E6%B1%9F%E8%8B%8F%E5%AE%9D%E5%8D%8E%E5%B1%B1%E5%9B%BD%E5%AE%B6%E6%A3%AE%E6%9E%97%E5%85%AC%E5%9B%AD?fromtitle=%E5%AE%9D%E5%8D%8E%E5%B1%B1%E5%9B%BD%E5%AE%B6%E6%A3%AE%E6%9E%97%E5%85%AC%E5%9B%AD&amp;fromid=10566126" /&gt;</v>
+        <v>&lt;Card CardID="20010015" CardType="01" CardName="宝华山国家森林公园" ScenicID="320206" Image="card_zhenjiang06" Text="宝华山国家森林公园介绍" Url="https://baike.baidu.com/item/%E6%B1%9F%E8%8B%8F%E5%AE%9D%E5%8D%8E%E5%B1%B1%E5%9B%BD%E5%AE%B6%E6%A3%AE%E6%9E%97%E5%85%AC%E5%9B%AD?fromtitle=%E5%AE%9D%E5%8D%8E%E5%B1%B1%E5%9B%BD%E5%AE%B6%E6%A3%AE%E6%9E%97%E5%85%AC%E5%9B%AD&amp;fromid=10566126" /&gt;</v>
       </c>
     </row>
     <row r="18" spans="1:8">
@@ -6326,7 +6307,7 @@
         <v>31</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>285</v>
+        <v>270</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>15</v>
@@ -6351,7 +6332,7 @@
         <v>32</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>286</v>
+        <v>271</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>25</v>
@@ -6365,7 +6346,7 @@
         <v>320101</v>
       </c>
       <c r="B3" s="24" t="s">
-        <v>281</v>
+        <v>266</v>
       </c>
       <c r="C3" s="6">
         <v>3201</v>
@@ -6380,7 +6361,7 @@
         <v>320102</v>
       </c>
       <c r="B4" s="24" t="s">
-        <v>281</v>
+        <v>266</v>
       </c>
       <c r="C4" s="6">
         <v>3201</v>
@@ -6395,7 +6376,7 @@
         <v>320103</v>
       </c>
       <c r="B5" s="24" t="s">
-        <v>281</v>
+        <v>266</v>
       </c>
       <c r="C5" s="6">
         <v>3201</v>
@@ -6410,7 +6391,7 @@
         <v>320104</v>
       </c>
       <c r="B6" s="24" t="s">
-        <v>281</v>
+        <v>266</v>
       </c>
       <c r="C6" s="6">
         <v>3201</v>
@@ -6425,7 +6406,7 @@
         <v>320105</v>
       </c>
       <c r="B7" s="24" t="s">
-        <v>281</v>
+        <v>266</v>
       </c>
       <c r="C7" s="6">
         <v>3201</v>
@@ -6440,7 +6421,7 @@
         <v>320106</v>
       </c>
       <c r="B8" s="24" t="s">
-        <v>281</v>
+        <v>266</v>
       </c>
       <c r="C8" s="6">
         <v>3201</v>
@@ -6455,7 +6436,7 @@
         <v>320107</v>
       </c>
       <c r="B9" s="24" t="s">
-        <v>281</v>
+        <v>266</v>
       </c>
       <c r="C9" s="6">
         <v>3201</v>
@@ -6470,7 +6451,7 @@
         <v>320108</v>
       </c>
       <c r="B10" s="24" t="s">
-        <v>281</v>
+        <v>266</v>
       </c>
       <c r="C10" s="6">
         <v>3201</v>
@@ -6485,7 +6466,7 @@
         <v>320109</v>
       </c>
       <c r="B11" s="24" t="s">
-        <v>281</v>
+        <v>266</v>
       </c>
       <c r="C11" s="6">
         <v>3201</v>
@@ -6500,7 +6481,7 @@
         <v>320201</v>
       </c>
       <c r="B12" s="24" t="s">
-        <v>281</v>
+        <v>266</v>
       </c>
       <c r="C12" s="6">
         <v>3202</v>
@@ -6515,7 +6496,7 @@
         <v>320202</v>
       </c>
       <c r="B13" s="24" t="s">
-        <v>281</v>
+        <v>266</v>
       </c>
       <c r="C13" s="6">
         <v>3202</v>
@@ -6530,7 +6511,7 @@
         <v>320203</v>
       </c>
       <c r="B14" s="24" t="s">
-        <v>281</v>
+        <v>266</v>
       </c>
       <c r="C14" s="6">
         <v>3202</v>
@@ -6545,7 +6526,7 @@
         <v>320204</v>
       </c>
       <c r="B15" s="24" t="s">
-        <v>281</v>
+        <v>266</v>
       </c>
       <c r="C15" s="6">
         <v>3202</v>
@@ -6560,7 +6541,7 @@
         <v>320205</v>
       </c>
       <c r="B16" s="24" t="s">
-        <v>281</v>
+        <v>266</v>
       </c>
       <c r="C16" s="6">
         <v>3202</v>
@@ -6575,7 +6556,7 @@
         <v>320206</v>
       </c>
       <c r="B17" s="24" t="s">
-        <v>281</v>
+        <v>266</v>
       </c>
       <c r="C17" s="6">
         <v>3202</v>
@@ -6615,7 +6596,7 @@
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" s="30" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="B1" s="30"/>
       <c r="C1" s="30"/>
@@ -6628,164 +6609,164 @@
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="23" t="s">
-        <v>224</v>
+        <v>209</v>
       </c>
       <c r="B2" s="23" t="s">
-        <v>225</v>
+        <v>210</v>
       </c>
       <c r="C2" s="23" t="s">
-        <v>226</v>
+        <v>211</v>
       </c>
       <c r="D2" s="23" t="s">
-        <v>227</v>
+        <v>212</v>
       </c>
       <c r="E2" s="23" t="s">
-        <v>228</v>
+        <v>213</v>
       </c>
       <c r="F2" s="23" t="s">
-        <v>229</v>
+        <v>214</v>
       </c>
       <c r="G2" s="23" t="s">
-        <v>230</v>
+        <v>215</v>
       </c>
       <c r="H2" s="23" t="s">
-        <v>231</v>
+        <v>216</v>
       </c>
       <c r="I2" s="23" t="s">
-        <v>232</v>
+        <v>217</v>
       </c>
       <c r="J2" s="23" t="s">
-        <v>233</v>
+        <v>218</v>
       </c>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="24" t="s">
-        <v>234</v>
+        <v>219</v>
       </c>
       <c r="B3" s="24" t="s">
-        <v>235</v>
+        <v>220</v>
       </c>
       <c r="C3" s="24" t="s">
-        <v>236</v>
+        <v>221</v>
       </c>
       <c r="D3" s="24" t="s">
-        <v>237</v>
+        <v>222</v>
       </c>
       <c r="E3" s="24" t="s">
-        <v>238</v>
+        <v>223</v>
       </c>
       <c r="F3" s="24" t="s">
-        <v>239</v>
+        <v>224</v>
       </c>
       <c r="G3" s="24" t="s">
-        <v>240</v>
+        <v>225</v>
       </c>
       <c r="H3" s="25" t="s">
-        <v>241</v>
+        <v>226</v>
       </c>
       <c r="I3" s="25" t="s">
-        <v>242</v>
+        <v>227</v>
       </c>
       <c r="J3" s="22" t="s">
-        <v>243</v>
+        <v>228</v>
       </c>
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="24" t="s">
-        <v>244</v>
+        <v>229</v>
       </c>
       <c r="B4" s="24" t="s">
-        <v>245</v>
+        <v>230</v>
       </c>
       <c r="C4" s="24" t="s">
-        <v>246</v>
+        <v>231</v>
       </c>
       <c r="D4" s="24" t="s">
-        <v>247</v>
+        <v>232</v>
       </c>
       <c r="E4" s="24" t="s">
-        <v>248</v>
+        <v>233</v>
       </c>
       <c r="H4" s="25" t="s">
-        <v>249</v>
+        <v>234</v>
       </c>
       <c r="I4" s="25" t="s">
-        <v>250</v>
+        <v>235</v>
       </c>
       <c r="J4" s="22" t="s">
-        <v>251</v>
+        <v>236</v>
       </c>
     </row>
     <row r="5" spans="1:11">
       <c r="A5" s="24" t="s">
-        <v>252</v>
+        <v>237</v>
       </c>
       <c r="B5" s="24" t="s">
-        <v>253</v>
+        <v>238</v>
       </c>
       <c r="C5" s="24" t="s">
-        <v>254</v>
+        <v>239</v>
       </c>
       <c r="D5" s="24" t="s">
-        <v>255</v>
+        <v>240</v>
       </c>
       <c r="E5" s="24" t="s">
-        <v>256</v>
+        <v>241</v>
       </c>
       <c r="F5" s="24" t="s">
-        <v>257</v>
+        <v>242</v>
       </c>
       <c r="G5" s="24" t="s">
-        <v>258</v>
+        <v>243</v>
       </c>
       <c r="H5" s="25" t="s">
-        <v>259</v>
+        <v>244</v>
       </c>
       <c r="I5" s="25" t="s">
-        <v>260</v>
+        <v>245</v>
       </c>
       <c r="J5" s="22" t="s">
-        <v>261</v>
+        <v>246</v>
       </c>
     </row>
     <row r="7" spans="1:11">
       <c r="A7" s="23" t="s">
-        <v>224</v>
+        <v>209</v>
       </c>
       <c r="B7" s="23" t="s">
-        <v>225</v>
+        <v>210</v>
       </c>
       <c r="C7" s="23" t="s">
-        <v>226</v>
+        <v>211</v>
       </c>
       <c r="D7" s="23" t="s">
-        <v>227</v>
+        <v>212</v>
       </c>
       <c r="E7" s="23" t="s">
-        <v>228</v>
+        <v>213</v>
       </c>
       <c r="F7" s="23" t="s">
-        <v>229</v>
+        <v>214</v>
       </c>
       <c r="G7" s="23" t="s">
-        <v>230</v>
+        <v>215</v>
       </c>
       <c r="H7" s="23" t="s">
-        <v>231</v>
+        <v>216</v>
       </c>
       <c r="I7" s="23" t="s">
-        <v>232</v>
+        <v>217</v>
       </c>
       <c r="J7" s="23" t="s">
-        <v>262</v>
+        <v>247</v>
       </c>
       <c r="K7" s="28" t="s">
-        <v>289</v>
+        <v>274</v>
       </c>
     </row>
     <row r="8" spans="1:11">
       <c r="A8" s="24" t="s">
-        <v>287</v>
+        <v>272</v>
       </c>
       <c r="K8" s="29" t="str">
         <f>"&lt;Question ID="""&amp;F8&amp;""" Count="""&amp;G8&amp;""" Scheme="""&amp;H8&amp;""" Source="""&amp;I8&amp;""" Score="""&amp;J8&amp;""" /&gt;"</f>
@@ -6825,42 +6806,42 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="31" t="s">
-        <v>263</v>
+        <v>248</v>
       </c>
       <c r="B1" s="31"/>
       <c r="C1" s="31"/>
       <c r="E1" s="32" t="s">
-        <v>264</v>
+        <v>249</v>
       </c>
       <c r="F1" s="33"/>
       <c r="G1" s="34"/>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="26" t="s">
-        <v>265</v>
+        <v>250</v>
       </c>
       <c r="B2" s="26" t="s">
-        <v>266</v>
+        <v>251</v>
       </c>
       <c r="C2" s="26" t="s">
-        <v>288</v>
+        <v>273</v>
       </c>
       <c r="E2" s="26" t="s">
-        <v>267</v>
+        <v>252</v>
       </c>
       <c r="F2" s="27" t="s">
-        <v>268</v>
+        <v>253</v>
       </c>
       <c r="G2" s="26" t="s">
-        <v>288</v>
+        <v>273</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="26" t="s">
-        <v>235</v>
+        <v>220</v>
       </c>
       <c r="B3" s="26" t="s">
-        <v>269</v>
+        <v>254</v>
       </c>
       <c r="C3" s="27" t="str">
         <f>"&lt;QuestionType ID="""&amp;A3&amp;""" Name="""&amp;B3&amp;""" /&gt;"</f>
@@ -6870,7 +6851,7 @@
         <v>0</v>
       </c>
       <c r="F3" s="27" t="s">
-        <v>270</v>
+        <v>255</v>
       </c>
       <c r="G3" s="27" t="str">
         <f>"&lt;Difficutly ID="""&amp;E3&amp;""" Name="""&amp;F3&amp;""" /&gt;"</f>
@@ -6879,10 +6860,10 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="26" t="s">
-        <v>271</v>
+        <v>256</v>
       </c>
       <c r="B4" s="26" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="C4" s="27" t="str">
         <f t="shared" ref="C4:C5" si="0">"&lt;QuestionType ID="""&amp;A4&amp;""" Name="""&amp;B4&amp;""" /&gt;"</f>
@@ -6892,7 +6873,7 @@
         <v>1</v>
       </c>
       <c r="F4" s="27" t="s">
-        <v>273</v>
+        <v>258</v>
       </c>
       <c r="G4" s="27" t="str">
         <f t="shared" ref="G4:G5" si="1">"&lt;Difficutly ID="""&amp;E4&amp;""" Name="""&amp;F4&amp;""" /&gt;"</f>
@@ -6901,10 +6882,10 @@
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="26" t="s">
-        <v>274</v>
+        <v>259</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>275</v>
+        <v>260</v>
       </c>
       <c r="C5" s="27" t="str">
         <f t="shared" si="0"/>
@@ -6914,7 +6895,7 @@
         <v>2</v>
       </c>
       <c r="F5" s="27" t="s">
-        <v>276</v>
+        <v>261</v>
       </c>
       <c r="G5" s="27" t="str">
         <f t="shared" si="1"/>
@@ -6923,39 +6904,39 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="23" t="s">
-        <v>291</v>
+        <v>276</v>
       </c>
       <c r="B8" s="23" t="s">
-        <v>277</v>
+        <v>262</v>
       </c>
       <c r="C8" s="23" t="s">
-        <v>278</v>
+        <v>263</v>
       </c>
       <c r="D8" s="23" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="E8" s="23" t="s">
-        <v>280</v>
+        <v>265</v>
       </c>
       <c r="F8" s="28" t="s">
-        <v>289</v>
+        <v>274</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="24" t="s">
-        <v>281</v>
+        <v>266</v>
       </c>
       <c r="B9" s="24" t="s">
-        <v>282</v>
+        <v>267</v>
       </c>
       <c r="C9" s="24" t="s">
-        <v>290</v>
+        <v>275</v>
       </c>
       <c r="D9" s="24" t="s">
-        <v>283</v>
+        <v>268</v>
       </c>
       <c r="E9" s="24" t="s">
-        <v>284</v>
+        <v>269</v>
       </c>
       <c r="F9" s="29" t="str">
         <f>"&lt;Scheme ID="""&amp;A9&amp;""" Count="""&amp;B9&amp;""" Matching="""&amp;C9&amp;""" Source="""&amp;D9&amp;""" Score="""&amp;E9&amp;""" /&gt;"</f>

</xml_diff>